<commit_message>
CIERRE 25 ENE 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE  HERRADURA  DICIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL#14  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE  HERRADURA  DICIEMBRE   2021.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL#14  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="A G O S T O    2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="386">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1480,6 +1480,9 @@
   </si>
   <si>
     <t>Delantales</t>
+  </si>
+  <si>
+    <t>diciembre</t>
   </si>
 </sst>
 </file>
@@ -3208,6 +3211,57 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3263,57 +3317,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5781,23 +5784,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="294"/>
-      <c r="C1" s="303" t="s">
+      <c r="B1" s="275"/>
+      <c r="C1" s="284" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="304"/>
-      <c r="E1" s="304"/>
-      <c r="F1" s="304"/>
-      <c r="G1" s="304"/>
-      <c r="H1" s="304"/>
-      <c r="I1" s="304"/>
-      <c r="J1" s="304"/>
-      <c r="K1" s="304"/>
-      <c r="L1" s="304"/>
-      <c r="M1" s="304"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="295"/>
+      <c r="B2" s="276"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -5807,17 +5810,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="277" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="278"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="279" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="279"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -5833,14 +5836,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -5850,10 +5853,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="288" t="s">
+      <c r="P4" s="269" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="289"/>
+      <c r="Q4" s="270"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7348,11 +7351,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="290">
+      <c r="M39" s="271">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="292">
+      <c r="N39" s="273">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -7384,8 +7387,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="291"/>
-      <c r="N40" s="293"/>
+      <c r="M40" s="272"/>
+      <c r="N40" s="274"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -7618,29 +7621,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="278" t="s">
+      <c r="H52" s="295" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="279"/>
+      <c r="I52" s="296"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="280">
+      <c r="K52" s="297">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="281"/>
-      <c r="M52" s="269">
+      <c r="L52" s="298"/>
+      <c r="M52" s="286">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="270"/>
+      <c r="N52" s="287"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="282" t="s">
+      <c r="D53" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="282"/>
+      <c r="E53" s="299"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -7651,22 +7654,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="283" t="s">
+      <c r="D54" s="300" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="283"/>
+      <c r="E54" s="300"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="284" t="s">
+      <c r="I54" s="301" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="285"/>
-      <c r="K54" s="286">
+      <c r="J54" s="302"/>
+      <c r="K54" s="303">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="287"/>
+      <c r="L54" s="304"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -7697,10 +7700,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="271">
-        <v>0</v>
-      </c>
-      <c r="L56" s="272"/>
+      <c r="K56" s="288">
+        <v>0</v>
+      </c>
+      <c r="L56" s="289"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -7717,22 +7720,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="273" t="s">
+      <c r="D58" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="274"/>
+      <c r="E58" s="291"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="275" t="s">
+      <c r="I58" s="292" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="276"/>
-      <c r="K58" s="277">
+      <c r="J58" s="293"/>
+      <c r="K58" s="294">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="277"/>
+      <c r="L58" s="294"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -7876,15 +7879,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -7896,6 +7890,15 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11459,23 +11462,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="294"/>
-      <c r="C1" s="303" t="s">
+      <c r="B1" s="275"/>
+      <c r="C1" s="284" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="304"/>
-      <c r="E1" s="304"/>
-      <c r="F1" s="304"/>
-      <c r="G1" s="304"/>
-      <c r="H1" s="304"/>
-      <c r="I1" s="304"/>
-      <c r="J1" s="304"/>
-      <c r="K1" s="304"/>
-      <c r="L1" s="304"/>
-      <c r="M1" s="304"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="295"/>
+      <c r="B2" s="276"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -11485,17 +11488,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="277" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="278"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="279" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="279"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -11511,14 +11514,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -11528,10 +11531,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="288" t="s">
+      <c r="P4" s="269" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="289"/>
+      <c r="Q4" s="270"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -13021,11 +13024,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="290">
+      <c r="M39" s="271">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="292">
+      <c r="N39" s="273">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -13051,8 +13054,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="291"/>
-      <c r="N40" s="293"/>
+      <c r="M40" s="272"/>
+      <c r="N40" s="274"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -13267,29 +13270,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="278" t="s">
+      <c r="H52" s="295" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="279"/>
+      <c r="I52" s="296"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="280">
+      <c r="K52" s="297">
         <f>I50+L50</f>
         <v>69642.26999999999</v>
       </c>
-      <c r="L52" s="281"/>
-      <c r="M52" s="269">
+      <c r="L52" s="298"/>
+      <c r="M52" s="286">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="270"/>
+      <c r="N52" s="287"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="282" t="s">
+      <c r="D53" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="282"/>
+      <c r="E53" s="299"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1505921.23</v>
@@ -13300,22 +13303,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="283" t="s">
+      <c r="D54" s="300" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="283"/>
+      <c r="E54" s="300"/>
       <c r="F54" s="102">
         <v>-1424333.95</v>
       </c>
-      <c r="I54" s="284" t="s">
+      <c r="I54" s="301" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="285"/>
-      <c r="K54" s="286">
+      <c r="J54" s="302"/>
+      <c r="K54" s="303">
         <f>F56+F57+F58</f>
         <v>222140.17000000004</v>
       </c>
-      <c r="L54" s="287"/>
+      <c r="L54" s="304"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -13346,11 +13349,11 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="271">
+      <c r="K56" s="288">
         <f>-C4</f>
         <v>-136234.76999999999</v>
       </c>
-      <c r="L56" s="272"/>
+      <c r="L56" s="289"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -13367,22 +13370,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="273" t="s">
+      <c r="D58" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="274"/>
+      <c r="E58" s="291"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="275" t="s">
+      <c r="I58" s="292" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="276"/>
-      <c r="K58" s="277">
+      <c r="J58" s="293"/>
+      <c r="K58" s="294">
         <f>K54+K56</f>
         <v>85905.400000000052</v>
       </c>
-      <c r="L58" s="277"/>
+      <c r="L58" s="294"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -13526,12 +13529,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -13546,6 +13543,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15169,23 +15172,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="294"/>
-      <c r="C1" s="303" t="s">
+      <c r="B1" s="275"/>
+      <c r="C1" s="284" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="304"/>
-      <c r="E1" s="304"/>
-      <c r="F1" s="304"/>
-      <c r="G1" s="304"/>
-      <c r="H1" s="304"/>
-      <c r="I1" s="304"/>
-      <c r="J1" s="304"/>
-      <c r="K1" s="304"/>
-      <c r="L1" s="304"/>
-      <c r="M1" s="304"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="295"/>
+      <c r="B2" s="276"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -15195,17 +15198,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="277" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="278"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="279" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="279"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -15221,14 +15224,14 @@
       <c r="D4" s="16">
         <v>44472</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -15238,10 +15241,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="288" t="s">
+      <c r="P4" s="269" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="289"/>
+      <c r="Q4" s="270"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -16816,11 +16819,11 @@
       <c r="L40" s="69">
         <v>1195.68</v>
       </c>
-      <c r="M40" s="290">
+      <c r="M40" s="271">
         <f>SUM(M5:M39)</f>
         <v>1982944.5</v>
       </c>
-      <c r="N40" s="292">
+      <c r="N40" s="273">
         <f>SUM(N5:N39)</f>
         <v>62048</v>
       </c>
@@ -16852,8 +16855,8 @@
       <c r="L41" s="69">
         <v>942.84</v>
       </c>
-      <c r="M41" s="291"/>
-      <c r="N41" s="293"/>
+      <c r="M41" s="272"/>
+      <c r="N41" s="274"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -17086,29 +17089,29 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="295" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="296"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="280">
+      <c r="K53" s="297">
         <f>I51+L51</f>
         <v>104139.16999999998</v>
       </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="269">
+      <c r="L53" s="298"/>
+      <c r="M53" s="286">
         <f>N40+M40</f>
         <v>2044992.5</v>
       </c>
-      <c r="N53" s="270"/>
+      <c r="N53" s="287"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="299"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
         <v>2004605.33</v>
@@ -17119,22 +17122,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="283" t="s">
+      <c r="D55" s="300" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="283"/>
+      <c r="E55" s="300"/>
       <c r="F55" s="102">
         <v>-2026393.17</v>
       </c>
-      <c r="I55" s="284" t="s">
+      <c r="I55" s="301" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="285"/>
-      <c r="K55" s="286">
+      <c r="J55" s="302"/>
+      <c r="K55" s="303">
         <f>F57+F58+F59</f>
         <v>178711.56000000014</v>
       </c>
-      <c r="L55" s="287"/>
+      <c r="L55" s="304"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -17165,11 +17168,11 @@
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="271">
+      <c r="K57" s="288">
         <f>-C4</f>
         <v>-134848.89000000001</v>
       </c>
-      <c r="L57" s="272"/>
+      <c r="L57" s="289"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -17186,22 +17189,22 @@
       <c r="C59" s="120">
         <v>44507</v>
       </c>
-      <c r="D59" s="273" t="s">
+      <c r="D59" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="274"/>
+      <c r="E59" s="291"/>
       <c r="F59" s="121">
         <v>192529.4</v>
       </c>
-      <c r="I59" s="275" t="s">
+      <c r="I59" s="292" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="276"/>
-      <c r="K59" s="277">
+      <c r="J59" s="293"/>
+      <c r="K59" s="294">
         <f>K55+K57</f>
         <v>43862.670000000129</v>
       </c>
-      <c r="L59" s="277"/>
+      <c r="L59" s="294"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -17345,12 +17348,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
@@ -17365,6 +17362,12 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19063,8 +19066,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView topLeftCell="H25" workbookViewId="0">
-      <selection activeCell="Q59" sqref="Q59"/>
+    <sheetView topLeftCell="E34" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19086,23 +19089,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="294"/>
-      <c r="C1" s="303" t="s">
+      <c r="B1" s="275"/>
+      <c r="C1" s="284" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="304"/>
-      <c r="E1" s="304"/>
-      <c r="F1" s="304"/>
-      <c r="G1" s="304"/>
-      <c r="H1" s="304"/>
-      <c r="I1" s="304"/>
-      <c r="J1" s="304"/>
-      <c r="K1" s="304"/>
-      <c r="L1" s="304"/>
-      <c r="M1" s="304"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="295"/>
+      <c r="B2" s="276"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -19112,17 +19115,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="277" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="278"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="279" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="279"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -19138,14 +19141,14 @@
       <c r="D4" s="16">
         <v>44507</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -19155,10 +19158,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="288" t="s">
+      <c r="P4" s="269" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="289"/>
+      <c r="Q4" s="270"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -20644,11 +20647,11 @@
       <c r="J40" s="67"/>
       <c r="K40" s="82"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="290">
+      <c r="M40" s="271">
         <f>SUM(M5:M39)</f>
         <v>1799884</v>
       </c>
-      <c r="N40" s="292">
+      <c r="N40" s="273">
         <f>SUM(N5:N39)</f>
         <v>38112</v>
       </c>
@@ -20674,8 +20677,8 @@
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="69"/>
-      <c r="M41" s="291"/>
-      <c r="N41" s="293"/>
+      <c r="M41" s="272"/>
+      <c r="N41" s="274"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -20890,29 +20893,29 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="295" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="296"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="280">
+      <c r="K53" s="297">
         <f>I51+L51</f>
         <v>62201.770000000004</v>
       </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="269">
+      <c r="L53" s="298"/>
+      <c r="M53" s="286">
         <f>N40+M40</f>
         <v>1837996</v>
       </c>
-      <c r="N53" s="270"/>
+      <c r="N53" s="287"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="299"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
         <v>1824289.23</v>
@@ -20923,22 +20926,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="283" t="s">
+      <c r="D55" s="300" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="283"/>
+      <c r="E55" s="300"/>
       <c r="F55" s="102">
         <v>-1751881.55</v>
       </c>
-      <c r="I55" s="284" t="s">
+      <c r="I55" s="301" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="285"/>
-      <c r="K55" s="286">
+      <c r="J55" s="302"/>
+      <c r="K55" s="303">
         <f>F57+F58+F59</f>
-        <v>81213.679999999935</v>
-      </c>
-      <c r="L55" s="287"/>
+        <v>270906.23999999993</v>
+      </c>
+      <c r="L55" s="304"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -20969,11 +20972,11 @@
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="271">
+      <c r="K57" s="288">
         <f>-C4</f>
         <v>-192529.4</v>
       </c>
-      <c r="L57" s="272"/>
+      <c r="L57" s="289"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -20990,22 +20993,22 @@
       <c r="C59" s="120">
         <v>44535</v>
       </c>
-      <c r="D59" s="273" t="s">
+      <c r="D59" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="274"/>
+      <c r="E59" s="291"/>
       <c r="F59" s="121">
-        <v>0</v>
-      </c>
-      <c r="I59" s="275" t="s">
+        <v>189692.56</v>
+      </c>
+      <c r="I59" s="292" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="276"/>
-      <c r="K59" s="277">
+      <c r="J59" s="293"/>
+      <c r="K59" s="294">
         <f>K55+K57</f>
-        <v>-111315.72000000006</v>
-      </c>
-      <c r="L59" s="277"/>
+        <v>78376.839999999938</v>
+      </c>
+      <c r="L59" s="294"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -21149,12 +21152,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
@@ -21169,6 +21166,12 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.15748031496062992" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22762,8 +22765,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22785,23 +22788,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="294"/>
-      <c r="C1" s="303" t="s">
+      <c r="B1" s="275"/>
+      <c r="C1" s="284" t="s">
         <v>322</v>
       </c>
-      <c r="D1" s="304"/>
-      <c r="E1" s="304"/>
-      <c r="F1" s="304"/>
-      <c r="G1" s="304"/>
-      <c r="H1" s="304"/>
-      <c r="I1" s="304"/>
-      <c r="J1" s="304"/>
-      <c r="K1" s="304"/>
-      <c r="L1" s="304"/>
-      <c r="M1" s="304"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="285"/>
+      <c r="F1" s="285"/>
+      <c r="G1" s="285"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
+      <c r="K1" s="285"/>
+      <c r="L1" s="285"/>
+      <c r="M1" s="285"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="295"/>
+      <c r="B2" s="276"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -22811,17 +22814,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="296" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="297"/>
+      <c r="B3" s="277" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="278"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="298" t="s">
+      <c r="H3" s="279" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="298"/>
+      <c r="I3" s="279"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -22832,19 +22835,19 @@
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="15">
-        <v>0</v>
+        <v>189692.56</v>
       </c>
       <c r="D4" s="16">
         <v>44535</v>
       </c>
-      <c r="E4" s="299" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="300"/>
-      <c r="H4" s="301" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="302"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -22854,10 +22857,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="288" t="s">
+      <c r="P4" s="269" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="289"/>
+      <c r="Q4" s="270"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -24326,9 +24329,15 @@
       <c r="G39" s="26"/>
       <c r="H39" s="32"/>
       <c r="I39" s="28"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="71"/>
-      <c r="L39" s="69"/>
+      <c r="J39" s="67" t="s">
+        <v>385</v>
+      </c>
+      <c r="K39" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39" s="69">
+        <v>549</v>
+      </c>
       <c r="M39" s="138">
         <v>0</v>
       </c>
@@ -24337,11 +24346,11 @@
       </c>
       <c r="P39" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>549</v>
       </c>
       <c r="Q39" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>549</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -24357,17 +24366,17 @@
       <c r="J40" s="67"/>
       <c r="K40" s="82"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="290">
+      <c r="M40" s="271">
         <f>SUM(M5:M39)</f>
         <v>2100554</v>
       </c>
-      <c r="N40" s="292">
+      <c r="N40" s="273">
         <f>SUM(N5:N39)</f>
         <v>70577</v>
       </c>
       <c r="P40" s="83">
         <f>SUM(P5:P39)</f>
-        <v>2396075.67</v>
+        <v>2396624.67</v>
       </c>
       <c r="Q40" s="222">
         <f>SUM(Q5:Q38)</f>
@@ -24387,8 +24396,8 @@
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="69"/>
-      <c r="M41" s="291"/>
-      <c r="N41" s="293"/>
+      <c r="M41" s="272"/>
+      <c r="N41" s="274"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -24585,7 +24594,7 @@
       </c>
       <c r="L51" s="101">
         <f>SUM(L5:L50)</f>
-        <v>116418.67</v>
+        <v>116967.67</v>
       </c>
       <c r="M51" s="102"/>
       <c r="N51" s="102"/>
@@ -24603,32 +24612,32 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="278" t="s">
+      <c r="H53" s="295" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="279"/>
+      <c r="I53" s="296"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="280">
+      <c r="K53" s="297">
         <f>I51+L51</f>
-        <v>119355.67</v>
-      </c>
-      <c r="L53" s="281"/>
-      <c r="M53" s="269">
+        <v>119904.67</v>
+      </c>
+      <c r="L53" s="298"/>
+      <c r="M53" s="286">
         <f>N40+M40</f>
         <v>2171131</v>
       </c>
-      <c r="N53" s="270"/>
+      <c r="N53" s="287"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="282" t="s">
+      <c r="D54" s="299" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="282"/>
+      <c r="E54" s="299"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
-        <v>2189465.33</v>
+        <v>2188916.33</v>
       </c>
       <c r="I54" s="108"/>
       <c r="J54" s="109"/>
@@ -24636,22 +24645,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="283" t="s">
+      <c r="D55" s="300" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="283"/>
+      <c r="E55" s="300"/>
       <c r="F55" s="102">
         <v>-2173697.9</v>
       </c>
-      <c r="I55" s="284" t="s">
+      <c r="I55" s="301" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="285"/>
-      <c r="K55" s="286">
+      <c r="J55" s="302"/>
+      <c r="K55" s="303">
         <f>F57+F58+F59</f>
-        <v>246233.13000000018</v>
-      </c>
-      <c r="L55" s="287"/>
+        <v>245684.13000000018</v>
+      </c>
+      <c r="L55" s="304"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -24675,18 +24684,18 @@
       </c>
       <c r="F57" s="102">
         <f>SUM(F54:F56)</f>
-        <v>15767.430000000168</v>
+        <v>15218.430000000168</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="271">
+      <c r="K57" s="288">
         <f>-C4</f>
-        <v>0</v>
-      </c>
-      <c r="L57" s="272"/>
+        <v>-189692.56</v>
+      </c>
+      <c r="L57" s="289"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -24703,22 +24712,22 @@
       <c r="C59" s="120">
         <v>44563</v>
       </c>
-      <c r="D59" s="273" t="s">
+      <c r="D59" s="290" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="274"/>
+      <c r="E59" s="291"/>
       <c r="F59" s="121">
         <v>221059.7</v>
       </c>
-      <c r="I59" s="275" t="s">
+      <c r="I59" s="292" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="276"/>
-      <c r="K59" s="277">
+      <c r="J59" s="293"/>
+      <c r="K59" s="294">
         <f>K55+K57</f>
-        <v>246233.13000000018</v>
-      </c>
-      <c r="L59" s="277"/>
+        <v>55991.570000000182</v>
+      </c>
+      <c r="L59" s="294"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -24862,6 +24871,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
@@ -24876,12 +24891,6 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>